<commit_message>
Edited script, removing images, includes the first scene completed. Adding some pictures. Removing some.
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
   <si>
     <t>Status</t>
   </si>
@@ -42,16 +42,179 @@
   </si>
   <si>
     <t xml:space="preserve">Team: Spell Shaded A01 </t>
+  </si>
+  <si>
+    <t>female_sassy.png</t>
+  </si>
+  <si>
+    <t>female_happy.png</t>
+  </si>
+  <si>
+    <t>Female is Happy and points at you</t>
+  </si>
+  <si>
+    <t>400x800px</t>
+  </si>
+  <si>
+    <t>http://danbooru.donmai.us/posts/696945</t>
+  </si>
+  <si>
+    <t>Placeholder</t>
+  </si>
+  <si>
+    <t>http://danbooru.donmai.us/posts/704147</t>
+  </si>
+  <si>
+    <t>Female is smiling, being a little sassy</t>
+  </si>
+  <si>
+    <t>olin.jpg</t>
+  </si>
+  <si>
+    <t>Olin Hall. Opening Scene</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Finished</t>
+  </si>
+  <si>
+    <t>goddard_lab.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goddard Lab room. </t>
+  </si>
+  <si>
+    <t>http://www.consigli.com/wp-content/assets/images/portfolio/colleges/wpi_top.jpg</t>
+  </si>
+  <si>
+    <t>goddardentrance.jpg</t>
+  </si>
+  <si>
+    <t>Goddard Lab Entrance</t>
+  </si>
+  <si>
+    <t>http://towers.wpi.edu/artimages/issues/2010-03-23/640/Goddardentrance.JPG</t>
+  </si>
+  <si>
+    <t>tryagain.png</t>
+  </si>
+  <si>
+    <t>tryagain2.png</t>
+  </si>
+  <si>
+    <t>First clip of placeholder</t>
+  </si>
+  <si>
+    <t>PLACEHOLDERONLY</t>
+  </si>
+  <si>
+    <t>Second clip of placeholder</t>
+  </si>
+  <si>
+    <t>female_angry.png</t>
+  </si>
+  <si>
+    <t>Female is angry.</t>
+  </si>
+  <si>
+    <t>female_sad.png</t>
+  </si>
+  <si>
+    <t>Female is sad</t>
+  </si>
+  <si>
+    <t>female_shocked.png</t>
+  </si>
+  <si>
+    <t>Female is shocked.</t>
+  </si>
+  <si>
+    <t>male_happy.png</t>
+  </si>
+  <si>
+    <t>Male is happy</t>
+  </si>
+  <si>
+    <t>male_sad.png</t>
+  </si>
+  <si>
+    <t>Male is sad</t>
+  </si>
+  <si>
+    <t>male_shocked.png</t>
+  </si>
+  <si>
+    <t>Male is shocked</t>
+  </si>
+  <si>
+    <t>male_angry.png</t>
+  </si>
+  <si>
+    <t>Male is angry</t>
+  </si>
+  <si>
+    <t>twin_happy.png</t>
+  </si>
+  <si>
+    <t>Twin is happy</t>
+  </si>
+  <si>
+    <t>Twin is sad</t>
+  </si>
+  <si>
+    <t>twin_sad.png</t>
+  </si>
+  <si>
+    <t>twin_shocked.png</t>
+  </si>
+  <si>
+    <t>twin_angry.png</t>
+  </si>
+  <si>
+    <t>Twin is shocked</t>
+  </si>
+  <si>
+    <t>Twin is angry</t>
+  </si>
+  <si>
+    <t>http://i34.tinypic.com/xl9iz7.jpg</t>
+  </si>
+  <si>
+    <t>tree.jpg</t>
+  </si>
+  <si>
+    <t>Picture of Tree outside Riley</t>
+  </si>
+  <si>
+    <t>1280x1080px</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -95,31 +258,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -132,9 +280,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -147,24 +293,26 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -445,14 +593,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.77734375" customWidth="1"/>
     <col min="2" max="2" width="50.77734375" customWidth="1"/>
     <col min="3" max="3" width="20.77734375" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" customWidth="1"/>
+    <col min="4" max="4" width="60.77734375" customWidth="1"/>
     <col min="5" max="5" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -461,57 +611,101 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="A5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="E6" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -521,32 +715,72 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
@@ -556,32 +790,64 @@
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
@@ -626,18 +892,38 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
@@ -647,32 +933,72 @@
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
@@ -696,7 +1022,17 @@
       <c r="E33" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D28" r:id="rId3"/>
+    <hyperlink ref="D29" r:id="rId4"/>
+    <hyperlink ref="D9" r:id="rId5"/>
+    <hyperlink ref="D10" r:id="rId6"/>
+    <hyperlink ref="D11" r:id="rId7"/>
+    <hyperlink ref="D12" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made separate file for scene two w/Jump in the original script. Made text type out instead of instant Added opening transitions
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
   <si>
     <t>Status</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>1280x1080px</t>
+  </si>
+  <si>
+    <t>dormroom.jpg</t>
+  </si>
+  <si>
+    <t>Picture of Male's Dormroom</t>
   </si>
 </sst>
 </file>
@@ -593,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,11 +1007,21 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>

</xml_diff>

<commit_message>
Made fantastic menu animation (for now.) And some edits to the first scene. Check them out!
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
   <si>
     <t>Status</t>
   </si>
@@ -195,6 +195,39 @@
   </si>
   <si>
     <t>Picture of Male's Dormroom</t>
+  </si>
+  <si>
+    <t>punch.mp3</t>
+  </si>
+  <si>
+    <t>Sound of a punch</t>
+  </si>
+  <si>
+    <t>1 sec</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=RHFN4-BLcIo</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>memento.mp3</t>
+  </si>
+  <si>
+    <t>Main Menu Music</t>
+  </si>
+  <si>
+    <t>3min:31sec</t>
+  </si>
+  <si>
+    <t>Composer: Myuu</t>
+  </si>
+  <si>
+    <t>main_menu.png</t>
+  </si>
+  <si>
+    <t>Main Menu Picture</t>
   </si>
 </sst>
 </file>
@@ -597,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,11 +896,19 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
@@ -1031,11 +1072,38 @@
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1047,8 +1115,9 @@
     <hyperlink ref="D10" r:id="rId6"/>
     <hyperlink ref="D11" r:id="rId7"/>
     <hyperlink ref="D12" r:id="rId8"/>
+    <hyperlink ref="D33" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some more definitions. Transitions. Placeholders. Added choices in SceneOne. Scene One should  be just about finished.
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
   <si>
     <t>Status</t>
   </si>
@@ -228,13 +228,16 @@
   </si>
   <si>
     <t>Main Menu Picture</t>
+  </si>
+  <si>
+    <t>http://www.renders-graphics.com/gallery/Angel-Beats-113,4/Nakamura-Yuri-Yuripp-83715.htm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +256,14 @@
     <font>
       <u/>
       <sz val="9"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -340,11 +351,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -632,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,19 +663,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
     </row>
@@ -702,47 +714,49 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="7" t="s">
+      <c r="C5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1089,19 +1103,19 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="8" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1116,8 +1130,9 @@
     <hyperlink ref="D11" r:id="rId7"/>
     <hyperlink ref="D12" r:id="rId8"/>
     <hyperlink ref="D33" r:id="rId9"/>
+    <hyperlink ref="D5" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tons of new changes. v1.2c +Unique Placeholders & SFX +Scene 2 and 3 +more in version
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="114">
   <si>
     <t>Status</t>
   </si>
@@ -191,9 +191,6 @@
     <t>1280x1080px</t>
   </si>
   <si>
-    <t>dormroom.jpg</t>
-  </si>
-  <si>
     <t>Picture of Male's Dormroom</t>
   </si>
   <si>
@@ -282,13 +279,100 @@
   </si>
   <si>
     <t>Need to Grab</t>
+  </si>
+  <si>
+    <t>https://s-media-cache-ak0.pinimg.com/736x/2a/2f/3d/2a2f3d76742ca581376e00bfd8e1ad05.jpg</t>
+  </si>
+  <si>
+    <t>http://img1.wikia.nocookie.net/__cb20110526080724/megamitensei/images/9/92/Male_01.png</t>
+  </si>
+  <si>
+    <t>Persona 3 Render http://i.imgur.com/xrTPwUz.png</t>
+  </si>
+  <si>
+    <t>http://orig03.deviantart.net/d66e/f/2012/137/1/a/arisato_minato_render_by_leobueno-d504erh.png</t>
+  </si>
+  <si>
+    <t>http://sieghartelsy.deviantart.com/art/Persona-3-Minato-Arisato-all-out-battle-render-464463156</t>
+  </si>
+  <si>
+    <t>http://redqueencoder.com/wp-content/uploads/2014/09/Angel-Beats.Yuri-Nakamura-Yurippe.640x960-5.jpg</t>
+  </si>
+  <si>
+    <t>http://orig12.deviantart.net/ec42/f/2011/092/4/b/p3p__arisato_minato_by_kurotsukiyomi-d3d0qk3.png</t>
+  </si>
+  <si>
+    <t>bg1.png</t>
+  </si>
+  <si>
+    <t>Part of Menu</t>
+  </si>
+  <si>
+    <t>Angel Beats Render</t>
+  </si>
+  <si>
+    <t>bg2.png</t>
+  </si>
+  <si>
+    <t>WPInL ve</t>
+  </si>
+  <si>
+    <t>672x660px</t>
+  </si>
+  <si>
+    <t>dorm.jpg</t>
+  </si>
+  <si>
+    <t>dramaticpunch.wav</t>
+  </si>
+  <si>
+    <t>Big Punch</t>
+  </si>
+  <si>
+    <t>idea.wav</t>
+  </si>
+  <si>
+    <t>When an idea emerges</t>
+  </si>
+  <si>
+    <t>menusound.wav</t>
+  </si>
+  <si>
+    <t>Button sound in Menu</t>
+  </si>
+  <si>
+    <t>objection.wav</t>
+  </si>
+  <si>
+    <t>For exclamations</t>
+  </si>
+  <si>
+    <t>save.wav</t>
+  </si>
+  <si>
+    <t>Sound for saving</t>
+  </si>
+  <si>
+    <t>sharp.wav</t>
+  </si>
+  <si>
+    <t>Shocked</t>
+  </si>
+  <si>
+    <t>Medium punch</t>
+  </si>
+  <si>
+    <t>whack.wav</t>
+  </si>
+  <si>
+    <t>Phoenix Wright SFX (ripped from game)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,6 +398,27 @@
     </font>
     <font>
       <u/>
+      <sz val="8"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -413,7 +518,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -422,8 +527,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -705,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B39" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,49 +885,51 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="8" t="s">
+      <c r="D6" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -840,8 +950,8 @@
       <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>51</v>
+      <c r="D9" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>11</v>
@@ -874,8 +984,8 @@
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>51</v>
+      <c r="D11" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>11</v>
@@ -891,8 +1001,8 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>51</v>
+      <c r="D12" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>11</v>
@@ -902,7 +1012,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -915,8 +1025,8 @@
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>51</v>
+      <c r="D14" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>11</v>
@@ -932,8 +1042,8 @@
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>51</v>
+      <c r="D15" s="4" t="s">
+        <v>85</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>11</v>
@@ -949,8 +1059,8 @@
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>51</v>
+      <c r="D16" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>11</v>
@@ -966,8 +1076,8 @@
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>51</v>
+      <c r="D17" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>11</v>
@@ -982,16 +1092,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>11</v>
@@ -999,30 +1109,54 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
@@ -1142,10 +1276,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>54</v>
@@ -1159,10 +1293,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>54</v>
@@ -1175,88 +1309,209 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="E33" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" s="9" t="s">
+      <c r="E34" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
+      <c r="B36" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="C36" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="D36" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="1" t="s">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="8" t="s">
+      <c r="B41" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="C41" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="D41" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>61</v>
+      <c r="E41" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" t="s">
+        <v>104</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" t="s">
+        <v>113</v>
+      </c>
+      <c r="E46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>109</v>
+      </c>
+      <c r="B47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" t="s">
+        <v>113</v>
+      </c>
+      <c r="E47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" t="s">
+        <v>113</v>
+      </c>
+      <c r="E48" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1265,18 +1520,15 @@
     <hyperlink ref="D4" r:id="rId2"/>
     <hyperlink ref="D28" r:id="rId3"/>
     <hyperlink ref="D29" r:id="rId4"/>
-    <hyperlink ref="D9" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId5" display="http://i34.tinypic.com/xl9iz7.jpg"/>
     <hyperlink ref="D10" r:id="rId6"/>
-    <hyperlink ref="D11" r:id="rId7"/>
-    <hyperlink ref="D12" r:id="rId8"/>
-    <hyperlink ref="D40" r:id="rId9"/>
-    <hyperlink ref="D5" r:id="rId10"/>
-    <hyperlink ref="D14" r:id="rId11"/>
-    <hyperlink ref="D15" r:id="rId12"/>
-    <hyperlink ref="D16" r:id="rId13"/>
-    <hyperlink ref="D17" r:id="rId14"/>
+    <hyperlink ref="D12" r:id="rId7"/>
+    <hyperlink ref="D40" r:id="rId8"/>
+    <hyperlink ref="D5" r:id="rId9"/>
+    <hyperlink ref="D16" r:id="rId10"/>
+    <hyperlink ref="D17" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major changes. Read Version.txt V1.4
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="119">
   <si>
     <t>Status</t>
   </si>
@@ -266,18 +266,9 @@
     <t>white.jpg</t>
   </si>
   <si>
-    <t>bigbang.mp4</t>
-  </si>
-  <si>
     <t>Video of chemical explosion</t>
   </si>
   <si>
-    <t>1080p(hopefully)</t>
-  </si>
-  <si>
-    <t>&lt;-----------&gt;</t>
-  </si>
-  <si>
     <t>Need to Grab</t>
   </si>
   <si>
@@ -366,6 +357,30 @@
   </si>
   <si>
     <t>Phoenix Wright SFX (ripped from game)</t>
+  </si>
+  <si>
+    <t>female_laughing.png</t>
+  </si>
+  <si>
+    <t>Female is laughing.</t>
+  </si>
+  <si>
+    <t>http://images6.fanpop.com/image/photos/33000000/Yuri-laughing-yuri-yurippe-nakamura-33002962-500-600.gif</t>
+  </si>
+  <si>
+    <t>quad.jpg</t>
+  </si>
+  <si>
+    <t>The Quad</t>
+  </si>
+  <si>
+    <t>boom.mp4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZJ7LbYBOntw</t>
+  </si>
+  <si>
+    <t>mpg</t>
   </si>
 </sst>
 </file>
@@ -813,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,7 +927,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>11</v>
@@ -934,41 +949,32 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>51</v>
+      <c r="D10" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
@@ -976,16 +982,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>86</v>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>11</v>
@@ -993,57 +999,57 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>91</v>
+      <c r="D12" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>11</v>
@@ -1051,16 +1057,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>11</v>
@@ -1068,126 +1074,126 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>9</v>
@@ -1200,41 +1206,41 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>20</v>
+      <c r="D28" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>17</v>
@@ -1242,16 +1248,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>17</v>
@@ -1259,16 +1265,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>16</v>
+      <c r="D30" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>17</v>
@@ -1276,10 +1282,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>98</v>
+        <v>14</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>54</v>
@@ -1288,15 +1294,15 @@
         <v>16</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>54</v>
@@ -1309,121 +1315,136 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="10" t="s">
+      <c r="A33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>17</v>
+      <c r="D33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>54</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="E35" s="10" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="C39" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B42" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C42" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D42" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E41" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" t="s">
-        <v>58</v>
-      </c>
-      <c r="D42" t="s">
-        <v>113</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="E42" s="9" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C43" t="s">
         <v>58</v>
       </c>
       <c r="D43" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E43" t="s">
         <v>60</v>
@@ -1431,16 +1452,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B44" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C44" t="s">
         <v>58</v>
       </c>
       <c r="D44" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E44" t="s">
         <v>60</v>
@@ -1448,16 +1469,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C45" t="s">
         <v>58</v>
       </c>
       <c r="D45" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E45" t="s">
         <v>60</v>
@@ -1465,16 +1486,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B46" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C46" t="s">
         <v>58</v>
       </c>
       <c r="D46" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E46" t="s">
         <v>60</v>
@@ -1482,16 +1503,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C47" t="s">
         <v>58</v>
       </c>
       <c r="D47" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
         <v>60</v>
@@ -1499,18 +1520,35 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B48" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C48" t="s">
         <v>58</v>
       </c>
       <c r="D48" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E48" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" t="s">
+        <v>110</v>
+      </c>
+      <c r="E49" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1518,15 +1556,15 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
     <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D28" r:id="rId3"/>
-    <hyperlink ref="D29" r:id="rId4"/>
-    <hyperlink ref="D9" r:id="rId5" display="http://i34.tinypic.com/xl9iz7.jpg"/>
-    <hyperlink ref="D10" r:id="rId6"/>
-    <hyperlink ref="D12" r:id="rId7"/>
-    <hyperlink ref="D40" r:id="rId8"/>
+    <hyperlink ref="D29" r:id="rId3"/>
+    <hyperlink ref="D30" r:id="rId4"/>
+    <hyperlink ref="D10" r:id="rId5" display="http://i34.tinypic.com/xl9iz7.jpg"/>
+    <hyperlink ref="D11" r:id="rId6"/>
+    <hyperlink ref="D13" r:id="rId7"/>
+    <hyperlink ref="D41" r:id="rId8"/>
     <hyperlink ref="D5" r:id="rId9"/>
-    <hyperlink ref="D16" r:id="rId10"/>
-    <hyperlink ref="D17" r:id="rId11"/>
+    <hyperlink ref="D17" r:id="rId10"/>
+    <hyperlink ref="D18" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId12"/>

</xml_diff>

<commit_message>
All put together. Menu has background. Some more animations have been added/fixed.
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="112">
   <si>
     <t>Status</t>
   </si>
@@ -86,33 +86,12 @@
     <t xml:space="preserve">Goddard Lab room. </t>
   </si>
   <si>
-    <t>http://www.consigli.com/wp-content/assets/images/portfolio/colleges/wpi_top.jpg</t>
-  </si>
-  <si>
     <t>goddardentrance.jpg</t>
   </si>
   <si>
     <t>Goddard Lab Entrance</t>
   </si>
   <si>
-    <t>http://towers.wpi.edu/artimages/issues/2010-03-23/640/Goddardentrance.JPG</t>
-  </si>
-  <si>
-    <t>tryagain.png</t>
-  </si>
-  <si>
-    <t>tryagain2.png</t>
-  </si>
-  <si>
-    <t>First clip of placeholder</t>
-  </si>
-  <si>
-    <t>PLACEHOLDERONLY</t>
-  </si>
-  <si>
-    <t>Second clip of placeholder</t>
-  </si>
-  <si>
     <t>female_angry.png</t>
   </si>
   <si>
@@ -221,9 +200,6 @@
     <t>Composer: Myuu</t>
   </si>
   <si>
-    <t>main_menu.png</t>
-  </si>
-  <si>
     <t>Main Menu Picture</t>
   </si>
   <si>
@@ -381,13 +357,16 @@
   </si>
   <si>
     <t>mpg</t>
+  </si>
+  <si>
+    <t>bg3.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -436,6 +415,12 @@
     <font>
       <sz val="8"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -533,7 +518,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -547,6 +532,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -830,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,16 +887,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>11</v>
@@ -918,16 +904,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>11</v>
@@ -935,10 +921,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>9</v>
@@ -950,31 +936,31 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
@@ -982,16 +968,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>11</v>
@@ -999,16 +985,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>11</v>
@@ -1016,16 +1002,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>11</v>
@@ -1040,16 +1026,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>11</v>
@@ -1057,16 +1043,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>11</v>
@@ -1074,16 +1060,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>11</v>
@@ -1091,16 +1077,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>11</v>
@@ -1115,16 +1101,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>11</v>
@@ -1132,16 +1118,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>17</v>
@@ -1149,16 +1135,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>11</v>
@@ -1166,13 +1152,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>16</v>
@@ -1189,38 +1175,18 @@
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
@@ -1231,13 +1197,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>16</v>
@@ -1254,30 +1220,30 @@
         <v>19</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>20</v>
+        <v>47</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1288,7 +1254,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>16</v>
@@ -1299,13 +1265,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>16</v>
@@ -1316,33 +1282,33 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>17</v>
@@ -1350,16 +1316,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E35" s="10" t="s">
         <v>17</v>
@@ -1367,33 +1333,33 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>11</v>
@@ -1401,163 +1367,163 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B43" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C43" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D43" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E43" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C44" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D44" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E44" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B45" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C45" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D45" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E45" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" t="s">
         <v>102</v>
       </c>
-      <c r="B46" t="s">
-        <v>103</v>
-      </c>
-      <c r="C46" t="s">
-        <v>58</v>
-      </c>
-      <c r="D46" t="s">
-        <v>110</v>
-      </c>
       <c r="E46" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B47" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D47" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E47" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C48" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D48" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E48" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D49" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E49" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
     <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D29" r:id="rId3"/>
-    <hyperlink ref="D30" r:id="rId4"/>
+    <hyperlink ref="D29" r:id="rId3" display="http://www.consigli.com/wp-content/assets/images/portfolio/colleges/wpi_top.jpg"/>
+    <hyperlink ref="D30" r:id="rId4" display="http://towers.wpi.edu/artimages/issues/2010-03-23/640/Goddardentrance.JPG"/>
     <hyperlink ref="D10" r:id="rId5" display="http://i34.tinypic.com/xl9iz7.jpg"/>
     <hyperlink ref="D11" r:id="rId6"/>
     <hyperlink ref="D13" r:id="rId7"/>

</xml_diff>

<commit_message>
Added in music for twin. Added credit screen. Smoothed out female and twin story a bit. Removed some placeholders.
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="115">
   <si>
     <t>Status</t>
   </si>
@@ -360,6 +360,15 @@
   </si>
   <si>
     <t>bg3.png</t>
+  </si>
+  <si>
+    <t>lament.mp3</t>
+  </si>
+  <si>
+    <t>Twin BGM</t>
+  </si>
+  <si>
+    <t>4min:10sec</t>
   </si>
 </sst>
 </file>
@@ -518,7 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -533,6 +542,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -814,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1400,28 +1410,28 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" t="s">
-        <v>102</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="A43" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" s="14" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C44" t="s">
         <v>51</v>
@@ -1435,10 +1445,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C45" t="s">
         <v>51</v>
@@ -1452,10 +1462,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
         <v>51</v>
@@ -1469,10 +1479,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
         <v>51</v>
@@ -1486,10 +1496,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
         <v>51</v>
@@ -1503,10 +1513,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C49" t="s">
         <v>51</v>
@@ -1515,6 +1525,23 @@
         <v>102</v>
       </c>
       <c r="E49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed scenes -> show
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="100">
   <si>
     <t>Status</t>
   </si>
@@ -44,9 +44,6 @@
     <t xml:space="preserve">Team: Spell Shaded A01 </t>
   </si>
   <si>
-    <t>female_sassy.png</t>
-  </si>
-  <si>
     <t>female_happy.png</t>
   </si>
   <si>
@@ -56,18 +53,9 @@
     <t>400x800px</t>
   </si>
   <si>
-    <t>http://danbooru.donmai.us/posts/696945</t>
-  </si>
-  <si>
     <t>Placeholder</t>
   </si>
   <si>
-    <t>http://danbooru.donmai.us/posts/704147</t>
-  </si>
-  <si>
-    <t>Female is smiling, being a little sassy</t>
-  </si>
-  <si>
     <t>olin.jpg</t>
   </si>
   <si>
@@ -158,9 +146,6 @@
     <t>Twin is angry</t>
   </si>
   <si>
-    <t>http://i34.tinypic.com/xl9iz7.jpg</t>
-  </si>
-  <si>
     <t>tree.jpg</t>
   </si>
   <si>
@@ -203,9 +188,6 @@
     <t>Main Menu Picture</t>
   </si>
   <si>
-    <t>http://www.renders-graphics.com/gallery/Angel-Beats-113,4/Nakamura-Yuri-Yuripp-83715.htm</t>
-  </si>
-  <si>
     <t>Original Animation</t>
   </si>
   <si>
@@ -248,27 +230,6 @@
     <t>Need to Grab</t>
   </si>
   <si>
-    <t>https://s-media-cache-ak0.pinimg.com/736x/2a/2f/3d/2a2f3d76742ca581376e00bfd8e1ad05.jpg</t>
-  </si>
-  <si>
-    <t>http://img1.wikia.nocookie.net/__cb20110526080724/megamitensei/images/9/92/Male_01.png</t>
-  </si>
-  <si>
-    <t>Persona 3 Render http://i.imgur.com/xrTPwUz.png</t>
-  </si>
-  <si>
-    <t>http://orig03.deviantart.net/d66e/f/2012/137/1/a/arisato_minato_render_by_leobueno-d504erh.png</t>
-  </si>
-  <si>
-    <t>http://sieghartelsy.deviantart.com/art/Persona-3-Minato-Arisato-all-out-battle-render-464463156</t>
-  </si>
-  <si>
-    <t>http://redqueencoder.com/wp-content/uploads/2014/09/Angel-Beats.Yuri-Nakamura-Yurippe.640x960-5.jpg</t>
-  </si>
-  <si>
-    <t>http://orig12.deviantart.net/ec42/f/2011/092/4/b/p3p__arisato_minato_by_kurotsukiyomi-d3d0qk3.png</t>
-  </si>
-  <si>
     <t>bg1.png</t>
   </si>
   <si>
@@ -335,15 +296,6 @@
     <t>Phoenix Wright SFX (ripped from game)</t>
   </si>
   <si>
-    <t>female_laughing.png</t>
-  </si>
-  <si>
-    <t>Female is laughing.</t>
-  </si>
-  <si>
-    <t>http://images6.fanpop.com/image/photos/33000000/Yuri-laughing-yuri-yurippe-nakamura-33002962-500-600.gif</t>
-  </si>
-  <si>
     <t>quad.jpg</t>
   </si>
   <si>
@@ -369,13 +321,16 @@
   </si>
   <si>
     <t>4min:10sec</t>
+  </si>
+  <si>
+    <t>Original - Janella</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,43 +341,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="9"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="8"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -527,22 +445,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -826,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -845,336 +760,319 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
+      <c r="D3" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
+      <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>11</v>
+      <c r="C6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>105</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>76</v>
+        <v>8</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>44</v>
+        <v>8</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>75</v>
+        <v>8</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>80</v>
+        <v>8</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="8"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>74</v>
+        <v>8</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>74</v>
+        <v>8</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>77</v>
+        <v>8</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>78</v>
+        <v>8</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>99</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1207,359 +1105,352 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>16</v>
+        <v>42</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>16</v>
+        <v>42</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
+      <c r="E35" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>11</v>
+      <c r="C39" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>53</v>
+      <c r="E42" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>53</v>
+      <c r="A43" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" t="s">
         <v>89</v>
       </c>
-      <c r="C44" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" t="s">
-        <v>102</v>
-      </c>
       <c r="E44" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D45" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E45" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C46" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D46" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E46" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C47" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E47" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E48" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C49" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E49" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D50" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E50" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D29" r:id="rId3" display="http://www.consigli.com/wp-content/assets/images/portfolio/colleges/wpi_top.jpg"/>
-    <hyperlink ref="D30" r:id="rId4" display="http://towers.wpi.edu/artimages/issues/2010-03-23/640/Goddardentrance.JPG"/>
-    <hyperlink ref="D10" r:id="rId5" display="http://i34.tinypic.com/xl9iz7.jpg"/>
-    <hyperlink ref="D11" r:id="rId6"/>
-    <hyperlink ref="D13" r:id="rId7"/>
-    <hyperlink ref="D41" r:id="rId8"/>
-    <hyperlink ref="D5" r:id="rId9"/>
-    <hyperlink ref="D17" r:id="rId10"/>
-    <hyperlink ref="D18" r:id="rId11"/>
+    <hyperlink ref="D3" r:id="rId1" display="http://danbooru.donmai.us/posts/696945"/>
+    <hyperlink ref="D29" r:id="rId2" display="http://www.consigli.com/wp-content/assets/images/portfolio/colleges/wpi_top.jpg"/>
+    <hyperlink ref="D30" r:id="rId3" display="http://towers.wpi.edu/artimages/issues/2010-03-23/640/Goddardentrance.JPG"/>
+    <hyperlink ref="D41" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId12"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Image maps for the game. :D
</commit_message>
<xml_diff>
--- a/Assets.xlsx
+++ b/Assets.xlsx
@@ -236,9 +236,6 @@
     <t>Part of Menu</t>
   </si>
   <si>
-    <t>Angel Beats Render</t>
-  </si>
-  <si>
     <t>bg2.png</t>
   </si>
   <si>
@@ -324,6 +321,9 @@
   </si>
   <si>
     <t>Original - Janella</t>
+  </si>
+  <si>
+    <t>Janella</t>
   </si>
 </sst>
 </file>
@@ -741,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,7 +787,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
@@ -804,7 +804,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>9</v>
@@ -821,7 +821,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>9</v>
@@ -838,7 +838,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>9</v>
@@ -868,7 +868,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>9</v>
@@ -885,7 +885,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>9</v>
@@ -902,7 +902,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>9</v>
@@ -919,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>9</v>
@@ -943,7 +943,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>9</v>
@@ -960,7 +960,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>9</v>
@@ -977,7 +977,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>9</v>
@@ -994,7 +994,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>9</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>53</v>
@@ -1032,7 +1032,7 @@
         <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>57</v>
@@ -1052,7 +1052,7 @@
         <v>42</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>9</v>
@@ -1060,10 +1060,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>42</v>
@@ -1173,7 +1173,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>43</v>
@@ -1241,10 +1241,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>42</v>
@@ -1258,16 +1258,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>9</v>
@@ -1309,13 +1309,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="C43" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>98</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>52</v>
@@ -1326,16 +1326,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" t="s">
         <v>75</v>
-      </c>
-      <c r="B44" t="s">
-        <v>76</v>
       </c>
       <c r="C44" t="s">
         <v>46</v>
       </c>
       <c r="D44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E44" t="s">
         <v>48</v>
@@ -1343,16 +1343,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" t="s">
         <v>77</v>
-      </c>
-      <c r="B45" t="s">
-        <v>78</v>
       </c>
       <c r="C45" t="s">
         <v>46</v>
       </c>
       <c r="D45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E45" t="s">
         <v>48</v>
@@ -1360,16 +1360,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" t="s">
         <v>79</v>
-      </c>
-      <c r="B46" t="s">
-        <v>80</v>
       </c>
       <c r="C46" t="s">
         <v>46</v>
       </c>
       <c r="D46" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E46" t="s">
         <v>48</v>
@@ -1377,16 +1377,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>80</v>
+      </c>
+      <c r="B47" t="s">
         <v>81</v>
-      </c>
-      <c r="B47" t="s">
-        <v>82</v>
       </c>
       <c r="C47" t="s">
         <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E47" t="s">
         <v>48</v>
@@ -1394,16 +1394,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" t="s">
         <v>83</v>
-      </c>
-      <c r="B48" t="s">
-        <v>84</v>
       </c>
       <c r="C48" t="s">
         <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E48" t="s">
         <v>48</v>
@@ -1411,16 +1411,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" t="s">
         <v>85</v>
-      </c>
-      <c r="B49" t="s">
-        <v>86</v>
       </c>
       <c r="C49" t="s">
         <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E49" t="s">
         <v>48</v>
@@ -1428,16 +1428,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" t="s">
         <v>46</v>
       </c>
       <c r="D50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E50" t="s">
         <v>48</v>

</xml_diff>